<commit_message>
Cambio nome main() di WithBox.py
</commit_message>
<xml_diff>
--- a/FilesOperations/a.xlsx
+++ b/FilesOperations/a.xlsx
@@ -914,10 +914,32 @@
           <t>2022-04-07</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>fsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>te</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>adex489</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2022-04-07</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nuovo codice</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ulteriore correzione non finita nella lista libri
</commit_message>
<xml_diff>
--- a/FilesOperations/a.xlsx
+++ b/FilesOperations/a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\LibraryProject\FilesOperations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C61E42-49C7-41DD-BB11-A714022BCA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40899CD8-126B-4846-A310-6B4A6A07B12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="2025" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListaLibri" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>TITOLO</t>
   </si>
@@ -40,6 +40,36 @@
     <t>SCUOLA</t>
   </si>
   <si>
+    <t>STATO</t>
+  </si>
+  <si>
+    <t>MATERIA</t>
+  </si>
+  <si>
+    <t>ANNO</t>
+  </si>
+  <si>
+    <t>Le avventure di Simoncino e Turbolinux</t>
+  </si>
+  <si>
+    <t>Simo &amp; Turmo</t>
+  </si>
+  <si>
+    <t>Aitek</t>
+  </si>
+  <si>
+    <t>X489</t>
+  </si>
+  <si>
+    <t>majorana</t>
+  </si>
+  <si>
+    <t>Perfetto</t>
+  </si>
+  <si>
+    <t>Informatica</t>
+  </si>
+  <si>
     <t>TopoPrincipe</t>
   </si>
   <si>
@@ -52,7 +82,7 @@
     <t>A100</t>
   </si>
   <si>
-    <t>majorana</t>
+    <t>Buono</t>
   </si>
   <si>
     <t>Il meraviglioso mago di Oz</t>
@@ -184,6 +214,12 @@
     <t>adex489</t>
   </si>
   <si>
+    <t>30/02/3000</t>
+  </si>
+  <si>
+    <t>08/04/2022</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
@@ -193,53 +229,41 @@
     <t>COGNOME</t>
   </si>
   <si>
+    <t>Adex</t>
+  </si>
+  <si>
+    <t>Simo</t>
+  </si>
+  <si>
     <t>Andres</t>
   </si>
   <si>
+    <t>passw1</t>
+  </si>
+  <si>
+    <t>1234simone</t>
+  </si>
+  <si>
     <t>Simone</t>
   </si>
   <si>
-    <t>passw1</t>
-  </si>
-  <si>
-    <t>1234simone</t>
-  </si>
-  <si>
     <t>passw2</t>
   </si>
   <si>
-    <t>Le avventure di Simoncino e Turbolinux</t>
-  </si>
-  <si>
-    <t>Simo &amp; Turmo</t>
-  </si>
-  <si>
-    <t>Aitek</t>
-  </si>
-  <si>
-    <t>X489</t>
-  </si>
-  <si>
-    <t>Adex</t>
-  </si>
-  <si>
-    <t>Simo</t>
-  </si>
-  <si>
-    <t>STATO</t>
-  </si>
-  <si>
-    <t>30/02/3000</t>
+    <t>adex490</t>
+  </si>
+  <si>
+    <t>adex491</t>
+  </si>
+  <si>
+    <t>adex492</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +275,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,7 +311,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -585,15 +614,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,210 +641,301 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="H10">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -824,7 +947,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,42 +957,147 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="4">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3">
         <v>44659</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -886,27 +1114,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -926,24 +1154,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>